<commit_message>
update to add v41 models, upgrade to R 4.3, and only consider models since the start of the daily tournament
</commit_message>
<xml_diff>
--- a/Optimize-Me.xlsx
+++ b/Optimize-Me.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/BVS/github/PUBLIC/vladthestaker_public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/BVS/github/PUBLIC/vladthestaker_PUBLIC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CA334-3AF6-A04C-8293-3D0D32C2ECD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE481B9E-BDAA-044B-ABFB-0134CBF6B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>ModelName</t>
   </si>
@@ -93,6 +93,30 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_CYRUS20</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_CAROLI20</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_XERXES20</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_SAM20</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_CYRUS60</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_CAROLI60</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_XERXES60</t>
+  </si>
+  <si>
+    <t>LG_LGBM_V41_SAM60</t>
   </si>
 </sst>
 </file>
@@ -418,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="178" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -450,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -464,7 +488,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3">
         <v>1000</v>
@@ -478,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C4">
         <v>1000</v>
@@ -492,7 +516,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C5">
         <v>1000</v>
@@ -506,7 +530,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C6">
         <v>1000</v>
@@ -520,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7">
         <v>1000</v>
@@ -534,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -548,7 +572,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9">
         <v>1000</v>
@@ -562,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10">
         <v>1000</v>
@@ -576,7 +600,7 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11">
         <v>1000</v>
@@ -590,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C12">
         <v>1000</v>
@@ -604,7 +628,7 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C13">
         <v>1000</v>
@@ -618,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C14">
         <v>1000</v>
@@ -632,12 +656,124 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15">
         <v>1000</v>
       </c>
       <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>339</v>
+      </c>
+      <c r="C16">
+        <v>1000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>339</v>
+      </c>
+      <c r="C17">
+        <v>1000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>339</v>
+      </c>
+      <c r="C18">
+        <v>1000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>339</v>
+      </c>
+      <c r="C19">
+        <v>1000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>339</v>
+      </c>
+      <c r="C20">
+        <v>1000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>339</v>
+      </c>
+      <c r="C21">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>339</v>
+      </c>
+      <c r="C22">
+        <v>1000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>339</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename round_offset column and update docs
Rename the grid offset column from round_offset_from_r843 to round_offset_from_base_round across code and outputs, and update related plots/labels. Adjusted step2_sweep_grid_windows.R and step3_build_3xportfolios_oos.R to read/write and reference the new column name (heatmap axis label, highlight tiles, cell key generation, and grid CSV I/O). Added AGENTS.md and bumped documentation: README.md revised for the new 3-step pipeline and CHANGELOG.md updated with V5.0.0 notes. Optimize-Me.xlsx was also updated and the output CSV header (output/step2-grid-window-sweep.csv) changed to the new column name.
</commit_message>
<xml_diff>
--- a/Optimize-Me.xlsx
+++ b/Optimize-Me.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/BVS/agents/numerai-vladthestaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D991AF7D-133B-744A-92C2-685612DC3900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93F12BE-9404-B241-AF29-E19AD0EBC427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="23580" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="16620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -248,16 +248,16 @@
     <t>Tweak as needed. Controls maximum training history per grid cell.</t>
   </si>
   <si>
-    <t>Tweak as needed. Higher values give stricter OOS validation reliability.</t>
-  </si>
-  <si>
-    <t>Tweak as needed. Higher values enforce denser round coverage.</t>
-  </si>
-  <si>
     <t>Tweak as needed. Stepsize for offset sweep. Larger step runs faster; smaller step searches more finely.</t>
   </si>
   <si>
     <t>Tweak as needed. Stepsize for windowsize sweep. Larger step runs faster; smaller step searches more finely.</t>
+  </si>
+  <si>
+    <t>Tweak as needed. Higher values gives a larger set of forward OOS validation rounds to evaluate the final models against.</t>
+  </si>
+  <si>
+    <t>Tweak as needed. Depending on how spotty model coverage is within a training window, the minimum number of models required affects the actual number of rounds on which is trained. Higher values (up to the total number of models in Optimize-Me) makes for more exclusions of rounds. Lower values makes for more exclusions of models from a training window.</t>
   </si>
 </sst>
 </file>
@@ -313,11 +313,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -903,16 +906,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
     <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" customWidth="1"/>
+    <col min="3" max="3" width="149.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -989,18 +992,18 @@
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>76</v>
+      <c r="C8" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1011,7 +1014,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1022,7 +1025,7 @@
         <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>